<commit_message>
Añadida Data de Burgoin
Redes en epanet modificadas para que se llene el tanque por los lodos
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="229">
   <si>
     <t>Fecha</t>
   </si>
@@ -1505,6 +1505,12 @@
   </si>
   <si>
     <t>big data description</t>
+  </si>
+  <si>
+    <t>https://core.ac.uk/download/pdf/41782666.pdf</t>
+  </si>
+  <si>
+    <t>Modelo matemático del sedimentador</t>
   </si>
 </sst>
 </file>
@@ -2157,7 +2163,7 @@
   <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3648,15 +3654,23 @@
       <c r="G73" s="19"/>
       <c r="H73" s="22"/>
     </row>
-    <row r="74" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="7">
         <v>73</v>
       </c>
       <c r="B74" s="19"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="19"/>
+      <c r="C74" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="D74" s="19">
+        <v>41782666</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>228</v>
+      </c>
       <c r="G74" s="19"/>
       <c r="H74" s="22"/>
     </row>

</xml_diff>

<commit_message>
Hasta Modelo de Conocimiento
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="328">
   <si>
     <t>Fecha</t>
   </si>
@@ -1753,6 +1753,112 @@
   <si>
     <t>libro acerca de automatizacio agua holones  
 NO CITABLE</t>
+  </si>
+  <si>
+    <t>No sirve</t>
+  </si>
+  <si>
+    <t>Estudios y Diseños Planta de Potabilización de Agua Centro Agropecuario Marengo</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S2351978917301610</t>
+  </si>
+  <si>
+    <t>digital twin</t>
+  </si>
+  <si>
+    <t>@article{uhlemann2017digital,
+  title={The digital twin: demonstrating the potential of real time data acquisition in production systems},
+  author={Uhlemann, Thomas H-J and Schock, Christoph and Lehmann, Christian and Freiberger, Stefan and Steinhilper, Rolf},
+  journal={Procedia Manufacturing},
+  volume={9},
+  pages={113--120},
+  year={2017},
+  publisher={Elsevier}
+}</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S2405896316325538</t>
+  </si>
+  <si>
+    <t>@article{schroeder2016digital,
+  title={Digital twin data modeling with automationml and a communication methodology for data exchange},
+  author={Schroeder, Greyce N and Steinmetz, Charles and Pereira, Carlos E and Espindola, Danubia B},
+  journal={IFAC-PapersOnLine},
+  volume={49},
+  number={30},
+  pages={12--17},
+  year={2016},
+  publisher={Elsevier}
+}</t>
+  </si>
+  <si>
+    <t>v31n1a05</t>
+  </si>
+  <si>
+    <t>Modelo de conocimiento</t>
+  </si>
+  <si>
+    <t>http://www.scielo.org.co/pdf/rib/v31n1/v31n1a05.pdf</t>
+  </si>
+  <si>
+    <t>https://repository.eafit.edu.co/bitstream/handle/10784/71/9588173736.pdf;sequence=1</t>
+  </si>
+  <si>
+    <t>Modelo de conocimiento ingeniero de conocimiento</t>
+  </si>
+  <si>
+    <t>Tesis Andres</t>
+  </si>
+  <si>
+    <t>http://eventos.saber.ula.ve/eventos/getFile.py/access?contribId=37&amp;sessionId=25&amp;resId=1&amp;materialId=paper&amp;confId=47</t>
+  </si>
+  <si>
+    <t>Modelo híbrido
+edgar chacón</t>
+  </si>
+  <si>
+    <t>CLCA_ifac_conf</t>
+  </si>
+  <si>
+    <t>http://amca.mx/memorias/amca2007/articulos/amca53.pdf?s_datos_Tema=3</t>
+  </si>
+  <si>
+    <t>sistemas hibridos</t>
+  </si>
+  <si>
+    <t>https://www.redalyc.org/pdf/849/84917310002.pdf</t>
+  </si>
+  <si>
+    <t>redes de petri</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/221922078_Online_Production_Scheduling_and_Re-Scheduling_in_Autonomous_Intelligent_Distributed_Environments</t>
+  </si>
+  <si>
+    <t>@inbook{inbook,
+author = {Chac�n, Edgar and Cardillo, Juan and Chac�n, Rafael and Zapata, Germán},
+year = {2012},
+month = {01},
+pages = {},
+title = {Online Production Scheduling and Re-Scheduling in Autonomous, Intelligent Distributed Environments},
+isbn = {978-953-307-935-6},
+doi = {10.5772/25933}
+}</t>
+  </si>
+  <si>
+    <t>Modelos de producción
+Holones
+Cadena de Valor</t>
+  </si>
+  <si>
+    <t>rtfiuz … 00002</t>
+  </si>
+  <si>
+    <t>Holones</t>
+  </si>
+  <si>
+    <t>http://ve.scielo.org/scielo.php?script=sci_arttext&amp;pid=S0254-07702009000100002</t>
   </si>
 </sst>
 </file>
@@ -2404,8 +2510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F101" sqref="F101"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2825,7 +2931,9 @@
       <c r="F19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="9"/>
+      <c r="G19" s="9" t="s">
+        <v>302</v>
+      </c>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.25">
@@ -3389,7 +3497,7 @@
       <c r="G46" s="19"/>
       <c r="H46" s="22"/>
     </row>
-    <row r="47" spans="1:9" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" s="21" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -3401,7 +3509,9 @@
       <c r="E47" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="F47" s="19"/>
+      <c r="F47" s="19" t="s">
+        <v>303</v>
+      </c>
       <c r="G47" s="19"/>
       <c r="H47" s="22"/>
     </row>
@@ -4412,51 +4522,75 @@
       </c>
       <c r="H100" s="22"/>
     </row>
-    <row r="101" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" s="21" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="7">
         <v>100</v>
       </c>
       <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="C101" s="19" t="s">
+        <v>304</v>
+      </c>
       <c r="D101" s="19"/>
       <c r="E101" s="19"/>
-      <c r="F101" s="19"/>
-      <c r="G101" s="19"/>
+      <c r="F101" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="G101" s="31" t="s">
+        <v>306</v>
+      </c>
       <c r="H101" s="22"/>
     </row>
-    <row r="102" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" s="21" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="7">
         <v>101</v>
       </c>
       <c r="B102" s="19"/>
-      <c r="C102" s="19"/>
+      <c r="C102" s="19" t="s">
+        <v>307</v>
+      </c>
       <c r="D102" s="19"/>
       <c r="E102" s="19"/>
-      <c r="F102" s="19"/>
-      <c r="G102" s="19"/>
+      <c r="F102" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="G102" s="31" t="s">
+        <v>308</v>
+      </c>
       <c r="H102" s="22"/>
     </row>
-    <row r="103" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="7">
         <v>102</v>
       </c>
       <c r="B103" s="19"/>
-      <c r="C103" s="19"/>
-      <c r="D103" s="19"/>
-      <c r="E103" s="19"/>
-      <c r="F103" s="19"/>
+      <c r="C103" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="D103" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="E103" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F103" s="19" t="s">
+        <v>310</v>
+      </c>
       <c r="G103" s="19"/>
       <c r="H103" s="22"/>
     </row>
-    <row r="104" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" s="21" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="7">
         <v>103</v>
       </c>
       <c r="B104" s="19"/>
-      <c r="C104" s="19"/>
+      <c r="C104" s="19" t="s">
+        <v>312</v>
+      </c>
       <c r="D104" s="19"/>
       <c r="E104" s="19"/>
-      <c r="F104" s="19"/>
+      <c r="F104" s="19" t="s">
+        <v>313</v>
+      </c>
       <c r="G104" s="19"/>
       <c r="H104" s="22"/>
     </row>
@@ -4468,68 +4602,98 @@
       <c r="C105" s="19"/>
       <c r="D105" s="19"/>
       <c r="E105" s="19"/>
-      <c r="F105" s="19"/>
+      <c r="F105" s="19" t="s">
+        <v>314</v>
+      </c>
       <c r="G105" s="19"/>
       <c r="H105" s="22"/>
     </row>
-    <row r="106" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" s="21" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="7">
         <v>105</v>
       </c>
       <c r="B106" s="19"/>
-      <c r="C106" s="19"/>
-      <c r="D106" s="19"/>
-      <c r="E106" s="19"/>
-      <c r="F106" s="19"/>
+      <c r="C106" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="D106" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="E106" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F106" s="19" t="s">
+        <v>316</v>
+      </c>
       <c r="G106" s="19"/>
       <c r="H106" s="22"/>
     </row>
-    <row r="107" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="7">
         <v>106</v>
       </c>
       <c r="B107" s="19"/>
-      <c r="C107" s="19"/>
+      <c r="C107" s="19" t="s">
+        <v>318</v>
+      </c>
       <c r="D107" s="19"/>
       <c r="E107" s="19"/>
-      <c r="F107" s="19"/>
+      <c r="F107" s="19" t="s">
+        <v>319</v>
+      </c>
       <c r="G107" s="19"/>
       <c r="H107" s="22"/>
     </row>
-    <row r="108" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="7">
         <v>107</v>
       </c>
       <c r="B108" s="19"/>
-      <c r="C108" s="19"/>
+      <c r="C108" s="19" t="s">
+        <v>320</v>
+      </c>
       <c r="D108" s="19"/>
       <c r="E108" s="19"/>
-      <c r="F108" s="19"/>
+      <c r="F108" s="19" t="s">
+        <v>321</v>
+      </c>
       <c r="G108" s="19"/>
       <c r="H108" s="22"/>
     </row>
-    <row r="109" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" s="21" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="7">
         <v>108</v>
       </c>
       <c r="B109" s="19"/>
-      <c r="C109" s="19"/>
+      <c r="C109" s="19" t="s">
+        <v>322</v>
+      </c>
       <c r="D109" s="19"/>
       <c r="E109" s="19"/>
-      <c r="F109" s="19"/>
-      <c r="G109" s="19"/>
+      <c r="F109" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="G109" s="31" t="s">
+        <v>323</v>
+      </c>
       <c r="H109" s="22"/>
     </row>
-    <row r="110" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" s="21" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="7">
         <v>109</v>
       </c>
       <c r="B110" s="19"/>
-      <c r="C110" s="19"/>
+      <c r="C110" s="19" t="s">
+        <v>327</v>
+      </c>
       <c r="D110" s="19"/>
       <c r="E110" s="19"/>
-      <c r="F110" s="19"/>
-      <c r="G110" s="19"/>
+      <c r="F110" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="G110" s="19" t="s">
+        <v>325</v>
+      </c>
       <c r="H110" s="22"/>
     </row>
     <row r="111" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Modelo de negocios hidrológicas
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="333">
   <si>
     <t>Fecha</t>
   </si>
@@ -1876,6 +1876,12 @@
   </si>
   <si>
     <t>HMS</t>
+  </si>
+  <si>
+    <t>https://www.murfreesborotn.gov/1583/Journey-to-The-Tap-How-Water-Gets-to-You</t>
+  </si>
+  <si>
+    <t>proceso agua</t>
   </si>
 </sst>
 </file>
@@ -2525,10 +2531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112:A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4735,15 +4741,21 @@
       </c>
       <c r="H111" s="22"/>
     </row>
-    <row r="112" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" s="21" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="7">
         <v>111</v>
       </c>
       <c r="B112" s="19"/>
-      <c r="C112" s="19"/>
+      <c r="C112" s="19" t="s">
+        <v>331</v>
+      </c>
       <c r="D112" s="19"/>
-      <c r="E112" s="19"/>
-      <c r="F112" s="19"/>
+      <c r="E112" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="F112" s="19" t="s">
+        <v>332</v>
+      </c>
       <c r="G112" s="19"/>
       <c r="H112" s="22"/>
     </row>
@@ -4770,6 +4782,306 @@
       <c r="F114" s="19"/>
       <c r="G114" s="19"/>
       <c r="H114" s="22"/>
+    </row>
+    <row r="115" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="7">
+        <v>114</v>
+      </c>
+      <c r="B115" s="19"/>
+      <c r="C115" s="19"/>
+      <c r="D115" s="19"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="19"/>
+      <c r="G115" s="19"/>
+      <c r="H115" s="22"/>
+    </row>
+    <row r="116" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="7">
+        <v>115</v>
+      </c>
+      <c r="B116" s="19"/>
+      <c r="C116" s="19"/>
+      <c r="D116" s="19"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="19"/>
+      <c r="G116" s="19"/>
+      <c r="H116" s="22"/>
+    </row>
+    <row r="117" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="7">
+        <v>116</v>
+      </c>
+      <c r="B117" s="19"/>
+      <c r="C117" s="19"/>
+      <c r="D117" s="19"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="19"/>
+      <c r="G117" s="19"/>
+      <c r="H117" s="22"/>
+    </row>
+    <row r="118" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="7">
+        <v>117</v>
+      </c>
+      <c r="B118" s="19"/>
+      <c r="C118" s="19"/>
+      <c r="D118" s="19"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
+      <c r="G118" s="19"/>
+      <c r="H118" s="22"/>
+    </row>
+    <row r="119" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="7">
+        <v>118</v>
+      </c>
+      <c r="B119" s="19"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="19"/>
+      <c r="E119" s="19"/>
+      <c r="F119" s="19"/>
+      <c r="G119" s="19"/>
+      <c r="H119" s="22"/>
+    </row>
+    <row r="120" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="7">
+        <v>119</v>
+      </c>
+      <c r="B120" s="19"/>
+      <c r="C120" s="19"/>
+      <c r="D120" s="19"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="19"/>
+      <c r="G120" s="19"/>
+      <c r="H120" s="22"/>
+    </row>
+    <row r="121" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="7">
+        <v>120</v>
+      </c>
+      <c r="B121" s="19"/>
+      <c r="C121" s="19"/>
+      <c r="D121" s="19"/>
+      <c r="E121" s="19"/>
+      <c r="F121" s="19"/>
+      <c r="G121" s="19"/>
+      <c r="H121" s="22"/>
+    </row>
+    <row r="122" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="7">
+        <v>121</v>
+      </c>
+      <c r="B122" s="19"/>
+      <c r="C122" s="19"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="19"/>
+      <c r="G122" s="19"/>
+      <c r="H122" s="22"/>
+    </row>
+    <row r="123" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="7">
+        <v>122</v>
+      </c>
+      <c r="B123" s="19"/>
+      <c r="C123" s="19"/>
+      <c r="D123" s="19"/>
+      <c r="E123" s="19"/>
+      <c r="F123" s="19"/>
+      <c r="G123" s="19"/>
+      <c r="H123" s="22"/>
+    </row>
+    <row r="124" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="7">
+        <v>123</v>
+      </c>
+      <c r="B124" s="19"/>
+      <c r="C124" s="19"/>
+      <c r="D124" s="19"/>
+      <c r="E124" s="19"/>
+      <c r="F124" s="19"/>
+      <c r="G124" s="19"/>
+      <c r="H124" s="22"/>
+    </row>
+    <row r="125" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="7">
+        <v>124</v>
+      </c>
+      <c r="B125" s="19"/>
+      <c r="C125" s="19"/>
+      <c r="D125" s="19"/>
+      <c r="E125" s="19"/>
+      <c r="F125" s="19"/>
+      <c r="G125" s="19"/>
+      <c r="H125" s="22"/>
+    </row>
+    <row r="126" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="7">
+        <v>125</v>
+      </c>
+      <c r="B126" s="19"/>
+      <c r="C126" s="19"/>
+      <c r="D126" s="19"/>
+      <c r="E126" s="19"/>
+      <c r="F126" s="19"/>
+      <c r="G126" s="19"/>
+      <c r="H126" s="22"/>
+    </row>
+    <row r="127" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="7">
+        <v>126</v>
+      </c>
+      <c r="B127" s="19"/>
+      <c r="C127" s="19"/>
+      <c r="D127" s="19"/>
+      <c r="E127" s="19"/>
+      <c r="F127" s="19"/>
+      <c r="G127" s="19"/>
+      <c r="H127" s="22"/>
+    </row>
+    <row r="128" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="7">
+        <v>127</v>
+      </c>
+      <c r="B128" s="19"/>
+      <c r="C128" s="19"/>
+      <c r="D128" s="19"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="19"/>
+      <c r="G128" s="19"/>
+      <c r="H128" s="22"/>
+    </row>
+    <row r="129" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="7">
+        <v>128</v>
+      </c>
+      <c r="B129" s="19"/>
+      <c r="C129" s="19"/>
+      <c r="D129" s="19"/>
+      <c r="E129" s="19"/>
+      <c r="F129" s="19"/>
+      <c r="G129" s="19"/>
+      <c r="H129" s="22"/>
+    </row>
+    <row r="130" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="7">
+        <v>129</v>
+      </c>
+      <c r="B130" s="19"/>
+      <c r="C130" s="19"/>
+      <c r="D130" s="19"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="19"/>
+      <c r="G130" s="19"/>
+      <c r="H130" s="22"/>
+    </row>
+    <row r="131" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="7">
+        <v>130</v>
+      </c>
+      <c r="B131" s="19"/>
+      <c r="C131" s="19"/>
+      <c r="D131" s="19"/>
+      <c r="E131" s="19"/>
+      <c r="F131" s="19"/>
+      <c r="G131" s="19"/>
+      <c r="H131" s="22"/>
+    </row>
+    <row r="132" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="7">
+        <v>131</v>
+      </c>
+      <c r="B132" s="19"/>
+      <c r="C132" s="19"/>
+      <c r="D132" s="19"/>
+      <c r="E132" s="19"/>
+      <c r="F132" s="19"/>
+      <c r="G132" s="19"/>
+      <c r="H132" s="22"/>
+    </row>
+    <row r="133" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="7">
+        <v>132</v>
+      </c>
+      <c r="B133" s="19"/>
+      <c r="C133" s="19"/>
+      <c r="D133" s="19"/>
+      <c r="E133" s="19"/>
+      <c r="F133" s="19"/>
+      <c r="G133" s="19"/>
+      <c r="H133" s="22"/>
+    </row>
+    <row r="134" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="7">
+        <v>133</v>
+      </c>
+      <c r="B134" s="19"/>
+      <c r="C134" s="19"/>
+      <c r="D134" s="19"/>
+      <c r="E134" s="19"/>
+      <c r="F134" s="19"/>
+      <c r="G134" s="19"/>
+      <c r="H134" s="22"/>
+    </row>
+    <row r="135" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="7">
+        <v>134</v>
+      </c>
+      <c r="B135" s="19"/>
+      <c r="C135" s="19"/>
+      <c r="D135" s="19"/>
+      <c r="E135" s="19"/>
+      <c r="F135" s="19"/>
+      <c r="G135" s="19"/>
+      <c r="H135" s="22"/>
+    </row>
+    <row r="136" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="7">
+        <v>135</v>
+      </c>
+      <c r="B136" s="19"/>
+      <c r="C136" s="19"/>
+      <c r="D136" s="19"/>
+      <c r="E136" s="19"/>
+      <c r="F136" s="19"/>
+      <c r="G136" s="19"/>
+      <c r="H136" s="22"/>
+    </row>
+    <row r="137" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="7">
+        <v>136</v>
+      </c>
+      <c r="B137" s="19"/>
+      <c r="C137" s="19"/>
+      <c r="D137" s="19"/>
+      <c r="E137" s="19"/>
+      <c r="F137" s="19"/>
+      <c r="G137" s="19"/>
+      <c r="H137" s="22"/>
+    </row>
+    <row r="138" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="7">
+        <v>137</v>
+      </c>
+      <c r="B138" s="19"/>
+      <c r="C138" s="19"/>
+      <c r="D138" s="19"/>
+      <c r="E138" s="19"/>
+      <c r="F138" s="19"/>
+      <c r="G138" s="19"/>
+      <c r="H138" s="22"/>
+    </row>
+    <row r="139" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="7">
+        <v>138</v>
+      </c>
+      <c r="B139" s="19"/>
+      <c r="C139" s="19"/>
+      <c r="D139" s="19"/>
+      <c r="E139" s="19"/>
+      <c r="F139" s="19"/>
+      <c r="G139" s="19"/>
+      <c r="H139" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Hidrológicas, sin detalle de potabilización
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -2533,8 +2533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112:A139"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Hasta prueba de jarras
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="335">
   <si>
     <t>Fecha</t>
   </si>
@@ -1882,6 +1882,12 @@
   </si>
   <si>
     <t>proceso agua</t>
+  </si>
+  <si>
+    <t>http://www.unicauca.edu.co/ai/publicaciones/Principios_de_programacion.pdf</t>
+  </si>
+  <si>
+    <t>PRINCIPIOS DE PROGRAMACIÓN Y CONTROL DE LA PRODUCCIÓN BAJO UN ENFOQUE HOLONICO</t>
   </si>
 </sst>
 </file>
@@ -2069,7 +2075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2161,6 +2167,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2533,8 +2542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F120" sqref="F120"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4759,15 +4768,19 @@
       <c r="G112" s="19"/>
       <c r="H112" s="22"/>
     </row>
-    <row r="113" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" s="21" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="7">
         <v>112</v>
       </c>
       <c r="B113" s="19"/>
-      <c r="C113" s="19"/>
+      <c r="C113" s="19" t="s">
+        <v>333</v>
+      </c>
       <c r="D113" s="19"/>
       <c r="E113" s="19"/>
-      <c r="F113" s="19"/>
+      <c r="F113" s="32" t="s">
+        <v>334</v>
+      </c>
       <c r="G113" s="19"/>
       <c r="H113" s="22"/>
     </row>

</xml_diff>

<commit_message>
Todos los cuadros de operación
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="342">
   <si>
     <t>Fecha</t>
   </si>
@@ -1903,6 +1903,12 @@
   </si>
   <si>
     <t>Operación y mantenimiento de plantas</t>
+  </si>
+  <si>
+    <t>http://www.tratamientodelagua.com.mx/sedimentadores-lamelares/</t>
+  </si>
+  <si>
+    <t>sedimentador laminar</t>
   </si>
 </sst>
 </file>
@@ -2557,8 +2563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4847,15 +4853,21 @@
       <c r="G116" s="19"/>
       <c r="H116" s="22"/>
     </row>
-    <row r="117" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="7">
         <v>116</v>
       </c>
       <c r="B117" s="19"/>
-      <c r="C117" s="19"/>
+      <c r="C117" s="19" t="s">
+        <v>340</v>
+      </c>
       <c r="D117" s="19"/>
-      <c r="E117" s="19"/>
-      <c r="F117" s="19"/>
+      <c r="E117" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="F117" s="19" t="s">
+        <v>341</v>
+      </c>
       <c r="G117" s="19"/>
       <c r="H117" s="22"/>
     </row>

</xml_diff>

<commit_message>
Descripción de las condiciones
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -2563,8 +2563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Dosis de coagulante en matlab
Simulación con la dosis y los sedimentadores de epanet
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="348">
   <si>
     <t>Fecha</t>
   </si>
@@ -899,16 +899,10 @@
     <t>trabalhoR</t>
   </si>
   <si>
-    <t>Modelo de tanques, diferentes tipologías de representación de tanques</t>
-  </si>
-  <si>
     <t>https://www.researchgate.net/publication/328410385_IAHR_AIIH_XXVIII_CONGRESO_LATINOAMERICANO_DE_HIDRAULICA_BUENOS_AIRES_ARGENTINA_SEPTIEMBRE_DE_2018_SIMULACION_DE_LA_OPERACION_DE_EMBALSES_MEDIANTE_EPANET_20</t>
   </si>
   <si>
     <t>Luis-Wilmer-Nieves</t>
-  </si>
-  <si>
-    <t>Modelo de embalses, aliviadero, etc. Prof luis mora</t>
   </si>
   <si>
     <t>http://www.bvsde.ops-oms.org/tecapro/documentos/agua/158esp-diseno-desare.pdf</t>
@@ -1909,6 +1903,30 @@
   </si>
   <si>
     <t>sedimentador laminar</t>
+  </si>
+  <si>
+    <t>Modelo de tanques, diferentes tipologías de representación de tanques con epanet</t>
+  </si>
+  <si>
+    <t>Modelo de embalses, aliviadero, etc. Prof luis mora. Epanet</t>
+  </si>
+  <si>
+    <t>nueve</t>
+  </si>
+  <si>
+    <t>FILTROS HERMOSO</t>
+  </si>
+  <si>
+    <t>http://www.ingenieroambiental.com/4014/nueve.pdf</t>
+  </si>
+  <si>
+    <t>http://dspace.ucuenca.edu.ec/bitstream/123456789/23369/1/tesis%20pdf.pdf</t>
+  </si>
+  <si>
+    <t>Velocidad de filtración, carrera de filtros, pruebas en campo, etc</t>
+  </si>
+  <si>
+    <t>La velocidad con que pasa el agua por el medio filtrante se mide como tasa de filtración o carga superficial (cociente entre el caudal q y el area filtrante)</t>
   </si>
 </sst>
 </file>
@@ -2563,8 +2581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2574,7 +2592,7 @@
     <col min="3" max="3" width="36.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="51.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="81.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
@@ -2985,7 +3003,7 @@
         <v>46</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H19" s="10"/>
     </row>
@@ -3563,7 +3581,7 @@
         <v>50</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G47" s="19"/>
       <c r="H47" s="22"/>
@@ -3747,7 +3765,7 @@
         <v>9</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>178</v>
+        <v>340</v>
       </c>
       <c r="G57" s="19"/>
       <c r="H57" s="22"/>
@@ -3758,16 +3776,16 @@
       </c>
       <c r="B58" s="19"/>
       <c r="C58" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" s="19" t="s">
         <v>179</v>
-      </c>
-      <c r="D58" s="19" t="s">
-        <v>180</v>
       </c>
       <c r="E58" s="19" t="s">
         <v>9</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>181</v>
+        <v>341</v>
       </c>
       <c r="G58" s="19"/>
       <c r="H58" s="22"/>
@@ -3778,16 +3796,16 @@
       </c>
       <c r="B59" s="19"/>
       <c r="C59" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D59" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E59" s="19" t="s">
         <v>9</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G59" s="19"/>
     </row>
@@ -3797,18 +3815,18 @@
       </c>
       <c r="B60" s="19"/>
       <c r="C60" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D60" s="19"/>
       <c r="E60" s="19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G60" s="19"/>
       <c r="H60" s="25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="21" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3817,20 +3835,20 @@
       </c>
       <c r="B61" s="19"/>
       <c r="C61" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="E61" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D61" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>192</v>
-      </c>
       <c r="F61" s="19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G61" s="19"/>
       <c r="H61" s="25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="21" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3839,16 +3857,16 @@
       </c>
       <c r="B62" s="19"/>
       <c r="C62" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D62" s="19"/>
       <c r="E62" s="19"/>
       <c r="F62" s="19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G62" s="19"/>
       <c r="H62" s="25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="21" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3857,16 +3875,16 @@
       </c>
       <c r="B63" s="19"/>
       <c r="C63" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="E63" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="D63" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>199</v>
-      </c>
       <c r="F63" s="19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G63" s="19"/>
       <c r="H63" s="22"/>
@@ -3877,20 +3895,20 @@
       </c>
       <c r="B64" s="19"/>
       <c r="C64" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D64" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G64" s="19"/>
       <c r="H64" s="22" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3899,19 +3917,19 @@
       </c>
       <c r="B65" s="19"/>
       <c r="C65" s="19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D65" s="19" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F65" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="G65" s="19" t="s">
         <v>205</v>
-      </c>
-      <c r="G65" s="19" t="s">
-        <v>207</v>
       </c>
       <c r="H65" s="22"/>
     </row>
@@ -3921,15 +3939,15 @@
       </c>
       <c r="B66" s="19"/>
       <c r="C66" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D66" s="19"/>
       <c r="E66" s="19"/>
       <c r="F66" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G66" s="19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H66" s="22"/>
     </row>
@@ -3939,17 +3957,17 @@
       </c>
       <c r="B67" s="19"/>
       <c r="C67" s="19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D67" s="19"/>
       <c r="E67" s="19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G67" s="19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H67" s="22"/>
     </row>
@@ -3962,10 +3980,10 @@
       <c r="D68" s="19"/>
       <c r="E68" s="19"/>
       <c r="F68" s="19" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G68" s="19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H68" s="22"/>
     </row>
@@ -3978,10 +3996,10 @@
       <c r="D69" s="19"/>
       <c r="E69" s="19"/>
       <c r="F69" s="19" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G69" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H69" s="22"/>
     </row>
@@ -3994,10 +4012,10 @@
       <c r="D70" s="19"/>
       <c r="E70" s="19"/>
       <c r="F70" s="19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G70" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H70" s="22"/>
     </row>
@@ -4008,13 +4026,13 @@
       <c r="B71" s="19"/>
       <c r="C71" s="19"/>
       <c r="D71" s="19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F71" s="19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G71" s="19"/>
       <c r="H71" s="22"/>
@@ -4025,16 +4043,16 @@
       </c>
       <c r="B72" s="19"/>
       <c r="C72" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="D72" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="D72" s="19" t="s">
-        <v>223</v>
-      </c>
       <c r="E72" s="19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F72" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G72" s="19"/>
       <c r="H72" s="22"/>
@@ -4045,16 +4063,16 @@
       </c>
       <c r="B73" s="19"/>
       <c r="C73" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="F73" s="19" t="s">
         <v>224</v>
-      </c>
-      <c r="D73" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="E73" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="F73" s="19" t="s">
-        <v>226</v>
       </c>
       <c r="G73" s="19"/>
       <c r="H73" s="22"/>
@@ -4065,16 +4083,16 @@
       </c>
       <c r="B74" s="19"/>
       <c r="C74" s="19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D74" s="19">
         <v>41782666</v>
       </c>
       <c r="E74" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F74" s="19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G74" s="19"/>
       <c r="H74" s="22"/>
@@ -4085,16 +4103,16 @@
       </c>
       <c r="B75" s="19"/>
       <c r="C75" s="19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D75" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F75" s="19" t="s">
         <v>229</v>
-      </c>
-      <c r="E75" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="F75" s="19" t="s">
-        <v>231</v>
       </c>
       <c r="G75" s="19"/>
       <c r="H75" s="22"/>
@@ -4105,16 +4123,16 @@
       </c>
       <c r="B76" s="19"/>
       <c r="C76" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F76" s="19" t="s">
         <v>232</v>
-      </c>
-      <c r="D76" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="E76" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="F76" s="19" t="s">
-        <v>234</v>
       </c>
       <c r="G76" s="19"/>
       <c r="H76" s="22"/>
@@ -4125,16 +4143,16 @@
       </c>
       <c r="B77" s="19"/>
       <c r="C77" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F77" s="19" t="s">
         <v>235</v>
-      </c>
-      <c r="D77" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="E77" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="F77" s="19" t="s">
-        <v>237</v>
       </c>
       <c r="G77" s="19"/>
       <c r="H77" s="22"/>
@@ -4145,16 +4163,16 @@
       </c>
       <c r="B78" s="19"/>
       <c r="C78" s="19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D78" s="19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E78" s="19" t="s">
         <v>9</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G78" s="19"/>
       <c r="H78" s="22"/>
@@ -4165,16 +4183,16 @@
       </c>
       <c r="B79" s="19"/>
       <c r="C79" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D79" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F79" s="19" t="s">
         <v>241</v>
-      </c>
-      <c r="E79" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="F79" s="19" t="s">
-        <v>243</v>
       </c>
       <c r="G79" s="19"/>
       <c r="H79" s="22"/>
@@ -4185,16 +4203,16 @@
       </c>
       <c r="B80" s="19"/>
       <c r="C80" s="19" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D80" s="19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E80" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G80" s="19"/>
       <c r="H80" s="22"/>
@@ -4205,19 +4223,19 @@
       </c>
       <c r="B81" s="19"/>
       <c r="C81" s="19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D81" s="19" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E81" s="19" t="s">
         <v>9</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G81" s="19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H81" s="22"/>
     </row>
@@ -4227,20 +4245,20 @@
       </c>
       <c r="B82" s="19"/>
       <c r="C82" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="D82" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F82" s="19" t="s">
         <v>251</v>
-      </c>
-      <c r="D82" s="19" t="s">
-        <v>252</v>
-      </c>
-      <c r="E82" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="F82" s="19" t="s">
-        <v>253</v>
       </c>
       <c r="G82" s="19"/>
       <c r="H82" s="25" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4249,16 +4267,16 @@
       </c>
       <c r="B83" s="19"/>
       <c r="C83" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D83" s="19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E83" s="19" t="s">
         <v>9</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G83" s="19"/>
       <c r="H83" s="22"/>
@@ -4269,19 +4287,19 @@
       </c>
       <c r="B84" s="19"/>
       <c r="C84" s="19" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D84" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E84" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F84" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="G84" s="19" t="s">
         <v>260</v>
-      </c>
-      <c r="G84" s="19" t="s">
-        <v>262</v>
       </c>
       <c r="H84" s="22"/>
     </row>
@@ -4291,12 +4309,12 @@
       </c>
       <c r="B85" s="19"/>
       <c r="C85" s="19" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D85" s="19"/>
       <c r="E85" s="19"/>
       <c r="F85" s="19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G85" s="19"/>
       <c r="H85" s="22"/>
@@ -4307,12 +4325,12 @@
       </c>
       <c r="B86" s="19"/>
       <c r="C86" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D86" s="19"/>
       <c r="E86" s="19"/>
       <c r="F86" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G86" s="19"/>
       <c r="H86" s="22"/>
@@ -4323,16 +4341,16 @@
       </c>
       <c r="B87" s="19"/>
       <c r="C87" s="19" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E87" s="19" t="s">
         <v>9</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G87" s="19"/>
       <c r="H87" s="22"/>
@@ -4343,16 +4361,16 @@
       </c>
       <c r="B88" s="19"/>
       <c r="C88" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E88" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G88" s="19"/>
       <c r="H88" s="22"/>
@@ -4363,12 +4381,12 @@
       </c>
       <c r="B89" s="19"/>
       <c r="C89" s="19" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D89" s="19"/>
       <c r="E89" s="19"/>
       <c r="F89" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G89" s="19"/>
       <c r="H89" s="22"/>
@@ -4379,12 +4397,12 @@
       </c>
       <c r="B90" s="19"/>
       <c r="C90" s="19" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D90" s="19"/>
       <c r="E90" s="19"/>
       <c r="F90" s="19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G90" s="19"/>
       <c r="H90" s="22"/>
@@ -4395,16 +4413,16 @@
       </c>
       <c r="B91" s="19"/>
       <c r="C91" s="19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D91" s="19" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E91" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F91" s="19" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G91" s="19"/>
       <c r="H91" s="22"/>
@@ -4415,12 +4433,12 @@
       </c>
       <c r="B92" s="19"/>
       <c r="C92" s="19" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D92" s="19"/>
       <c r="E92" s="19"/>
       <c r="F92" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G92" s="19"/>
       <c r="H92" s="22"/>
@@ -4431,12 +4449,12 @@
       </c>
       <c r="B93" s="19"/>
       <c r="C93" s="19" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D93" s="19"/>
       <c r="E93" s="19"/>
       <c r="F93" s="19" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G93" s="19"/>
       <c r="H93" s="22"/>
@@ -4447,19 +4465,19 @@
       </c>
       <c r="B94" s="19"/>
       <c r="C94" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="D94" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="E94" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F94" s="19" t="s">
         <v>280</v>
       </c>
-      <c r="D94" s="19" t="s">
+      <c r="G94" s="19" t="s">
         <v>281</v>
-      </c>
-      <c r="E94" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="F94" s="19" t="s">
-        <v>282</v>
-      </c>
-      <c r="G94" s="19" t="s">
-        <v>283</v>
       </c>
       <c r="H94" s="22"/>
     </row>
@@ -4469,16 +4487,16 @@
       </c>
       <c r="B95" s="19"/>
       <c r="C95" s="19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D95" s="19"/>
       <c r="E95" s="19"/>
       <c r="F95" s="19" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G95" s="19"/>
       <c r="H95" s="22" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="96" spans="1:8" s="21" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4487,12 +4505,12 @@
       </c>
       <c r="B96" s="19"/>
       <c r="C96" s="19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D96" s="19"/>
       <c r="E96" s="19"/>
       <c r="F96" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G96" s="19"/>
       <c r="H96" s="22"/>
@@ -4503,14 +4521,14 @@
       </c>
       <c r="B97" s="19"/>
       <c r="C97" s="19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D97" s="19"/>
       <c r="E97" s="19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F97" s="19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G97" s="19"/>
       <c r="H97" s="22"/>
@@ -4520,18 +4538,18 @@
         <v>97</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D98" s="19"/>
       <c r="E98" s="19"/>
       <c r="F98" s="19" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G98" s="31" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H98" s="22"/>
     </row>
@@ -4540,15 +4558,15 @@
         <v>98</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C99" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D99" s="19"/>
       <c r="E99" s="19"/>
       <c r="F99" s="19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G99" s="19"/>
       <c r="H99" s="22"/>
@@ -4559,19 +4577,19 @@
       </c>
       <c r="B100" s="19"/>
       <c r="C100" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D100" s="19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E100" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F100" s="19" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G100" s="31" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H100" s="22"/>
     </row>
@@ -4581,15 +4599,15 @@
       </c>
       <c r="B101" s="19"/>
       <c r="C101" s="19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D101" s="19"/>
       <c r="E101" s="19"/>
       <c r="F101" s="19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G101" s="31" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H101" s="22"/>
     </row>
@@ -4599,15 +4617,15 @@
       </c>
       <c r="B102" s="19"/>
       <c r="C102" s="19" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D102" s="19"/>
       <c r="E102" s="19"/>
       <c r="F102" s="19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G102" s="31" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H102" s="22"/>
     </row>
@@ -4617,16 +4635,16 @@
       </c>
       <c r="B103" s="19"/>
       <c r="C103" s="19" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E103" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F103" s="19" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G103" s="19"/>
       <c r="H103" s="22"/>
@@ -4637,12 +4655,12 @@
       </c>
       <c r="B104" s="19"/>
       <c r="C104" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D104" s="19"/>
       <c r="E104" s="19"/>
       <c r="F104" s="19" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G104" s="19"/>
       <c r="H104" s="22"/>
@@ -4656,7 +4674,7 @@
       <c r="D105" s="19"/>
       <c r="E105" s="19"/>
       <c r="F105" s="19" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G105" s="19"/>
       <c r="H105" s="22"/>
@@ -4667,16 +4685,16 @@
       </c>
       <c r="B106" s="19"/>
       <c r="C106" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="D106" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="D106" s="19" t="s">
-        <v>317</v>
-      </c>
       <c r="E106" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F106" s="19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G106" s="19"/>
       <c r="H106" s="22"/>
@@ -4687,12 +4705,12 @@
       </c>
       <c r="B107" s="19"/>
       <c r="C107" s="19" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D107" s="19"/>
       <c r="E107" s="19"/>
       <c r="F107" s="19" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G107" s="19"/>
       <c r="H107" s="22"/>
@@ -4703,12 +4721,12 @@
       </c>
       <c r="B108" s="19"/>
       <c r="C108" s="19" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D108" s="19"/>
       <c r="E108" s="19"/>
       <c r="F108" s="19" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G108" s="19"/>
       <c r="H108" s="22"/>
@@ -4719,15 +4737,15 @@
       </c>
       <c r="B109" s="19"/>
       <c r="C109" s="19" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D109" s="19"/>
       <c r="E109" s="19"/>
       <c r="F109" s="19" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G109" s="31" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H109" s="22"/>
     </row>
@@ -4737,15 +4755,15 @@
       </c>
       <c r="B110" s="19"/>
       <c r="C110" s="19" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D110" s="19"/>
       <c r="E110" s="19"/>
       <c r="F110" s="19" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G110" s="19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H110" s="22"/>
     </row>
@@ -4755,19 +4773,19 @@
       </c>
       <c r="B111" s="19"/>
       <c r="C111" s="19" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D111" s="19" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E111" s="19" t="s">
         <v>50</v>
       </c>
       <c r="F111" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="G111" s="31" t="s">
         <v>326</v>
-      </c>
-      <c r="G111" s="31" t="s">
-        <v>328</v>
       </c>
       <c r="H111" s="22"/>
     </row>
@@ -4777,14 +4795,14 @@
       </c>
       <c r="B112" s="19"/>
       <c r="C112" s="19" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D112" s="19"/>
       <c r="E112" s="19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F112" s="19" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G112" s="19"/>
       <c r="H112" s="22"/>
@@ -4795,12 +4813,12 @@
       </c>
       <c r="B113" s="19"/>
       <c r="C113" s="19" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D113" s="19"/>
       <c r="E113" s="19"/>
       <c r="F113" s="32" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G113" s="19"/>
       <c r="H113" s="22"/>
@@ -4811,12 +4829,12 @@
       </c>
       <c r="B114" s="19"/>
       <c r="C114" s="19" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D114" s="19"/>
       <c r="E114" s="19"/>
       <c r="F114" s="19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G114" s="19"/>
       <c r="H114" s="22"/>
@@ -4827,12 +4845,12 @@
       </c>
       <c r="B115" s="19"/>
       <c r="C115" s="19" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D115" s="19"/>
       <c r="E115" s="19"/>
       <c r="F115" s="19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G115" s="19"/>
       <c r="H115" s="22"/>
@@ -4843,12 +4861,12 @@
       </c>
       <c r="B116" s="19"/>
       <c r="C116" s="19" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D116" s="19"/>
       <c r="E116" s="19"/>
       <c r="F116" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G116" s="19"/>
       <c r="H116" s="22"/>
@@ -4859,51 +4877,67 @@
       </c>
       <c r="B117" s="19"/>
       <c r="C117" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D117" s="19"/>
       <c r="E117" s="19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F117" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G117" s="19"/>
       <c r="H117" s="22"/>
     </row>
-    <row r="118" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="7">
         <v>117</v>
       </c>
       <c r="B118" s="19"/>
-      <c r="C118" s="19"/>
-      <c r="D118" s="19"/>
-      <c r="E118" s="19"/>
-      <c r="F118" s="19"/>
+      <c r="C118" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="D118" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="E118" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F118" s="19" t="s">
+        <v>343</v>
+      </c>
       <c r="G118" s="19"/>
       <c r="H118" s="22"/>
     </row>
-    <row r="119" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" s="21" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="7">
         <v>118</v>
       </c>
       <c r="B119" s="19"/>
-      <c r="C119" s="19"/>
+      <c r="C119" s="19" t="s">
+        <v>345</v>
+      </c>
       <c r="D119" s="19"/>
       <c r="E119" s="19"/>
-      <c r="F119" s="19"/>
+      <c r="F119" s="19" t="s">
+        <v>346</v>
+      </c>
       <c r="G119" s="19"/>
       <c r="H119" s="22"/>
     </row>
-    <row r="120" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" s="21" customFormat="1" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="7">
         <v>119</v>
       </c>
       <c r="B120" s="19"/>
-      <c r="C120" s="19"/>
+      <c r="C120" s="19" t="s">
+        <v>233</v>
+      </c>
       <c r="D120" s="19"/>
       <c r="E120" s="19"/>
-      <c r="F120" s="19"/>
+      <c r="F120" s="19" t="s">
+        <v>347</v>
+      </c>
       <c r="G120" s="19"/>
       <c r="H120" s="22"/>
     </row>

</xml_diff>

<commit_message>
Modificación de antecedentes, intro e implementación
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="379">
   <si>
     <t>Fecha</t>
   </si>
@@ -1966,6 +1966,81 @@
   </si>
   <si>
     <t>modelo dosis neural net</t>
+  </si>
+  <si>
+    <t>https://prodindu.wordpress.com/revolucion-industrial-4-0/</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>cuarta-revoluc</t>
+  </si>
+  <si>
+    <t>http://sci-hub.tw/https://doi.org/10.1002/j.1551-8833.2006.tb07609.x</t>
+  </si>
+  <si>
+    <t>water trough the years</t>
+  </si>
+  <si>
+    <t>pericles_....3398</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Mays, Larry and Koutsoyiannis, Demetris and Angelakis, A.},
+year = {2007},
+month = {03},
+pages = {},
+title = {A brief history of urban water supply in antiquity},
+volume = {7},
+journal = {Water Science &amp; Technology: Water Supply},
+doi = {10.2166/ws.2007.001}
+}</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/228350050_A_brief_history_of_urban_water_supply_in_antiquity</t>
+  </si>
+  <si>
+    <t>Historia del agua antigua grecia</t>
+  </si>
+  <si>
+    <t>39309-Texto del artículo-48399-2-10-20120628</t>
+  </si>
+  <si>
+    <t>Aguaa evolucion plantas tratamiento</t>
+  </si>
+  <si>
+    <t>Lofrano , G. y Brown , J. (2010). Wastewater management through the ages: A
+history of mankind, Science of the Total Environment, 408, 5254 – 5264.</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Lofrano, Giusy and Brown, Jeanette},
+year = {2010},
+month = {10},
+pages = {5254-64},
+title = {Wastewater Management through the Ages: A History of Mankind},
+volume = {408},
+journal = {The Science of the total environment},
+doi = {10.1016/j.scitotenv.2010.07.062}
+}</t>
+  </si>
+  <si>
+    <t>Cooper , P.F. (2007). Historical aspects of wastewater treatment. In: Lens, P., Seeman,
+G., Lettinga, G. (eds). Decentralised sanitation and reuse: concepts, systems
+and implementation. IWA Publishing.</t>
+  </si>
+  <si>
+    <t>http://www.bvsde.paho.org/bvsacd/leeds/cooper.pdf</t>
+  </si>
+  <si>
+    <t>toda la evolucion de agua</t>
+  </si>
+  <si>
+    <t>UPS-CT005251</t>
+  </si>
+  <si>
+    <t>Mariela redes etc</t>
   </si>
 </sst>
 </file>
@@ -2620,8 +2695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5094,65 +5169,99 @@
       <c r="G127" s="19"/>
       <c r="H127" s="22"/>
     </row>
-    <row r="128" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="7">
         <v>127</v>
       </c>
       <c r="B128" s="19"/>
-      <c r="C128" s="19"/>
-      <c r="D128" s="19"/>
-      <c r="E128" s="19"/>
+      <c r="C128" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="D128" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="E128" s="19" t="s">
+        <v>362</v>
+      </c>
       <c r="F128" s="19"/>
       <c r="G128" s="19"/>
       <c r="H128" s="22"/>
     </row>
-    <row r="129" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" s="21" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="7">
         <v>128</v>
       </c>
       <c r="B129" s="19"/>
-      <c r="C129" s="19"/>
+      <c r="C129" s="19" t="s">
+        <v>364</v>
+      </c>
       <c r="D129" s="19"/>
       <c r="E129" s="19"/>
-      <c r="F129" s="19"/>
-      <c r="G129" s="19"/>
+      <c r="F129" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="G129" s="19" t="s">
+        <v>366</v>
+      </c>
       <c r="H129" s="22"/>
     </row>
-    <row r="130" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" s="21" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="7">
         <v>129</v>
       </c>
       <c r="B130" s="19"/>
-      <c r="C130" s="19"/>
+      <c r="C130" s="19" t="s">
+        <v>368</v>
+      </c>
       <c r="D130" s="19"/>
       <c r="E130" s="19"/>
-      <c r="F130" s="19"/>
-      <c r="G130" s="19"/>
+      <c r="F130" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="G130" s="31" t="s">
+        <v>367</v>
+      </c>
       <c r="H130" s="22"/>
     </row>
-    <row r="131" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" s="21" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="7">
         <v>130</v>
       </c>
       <c r="B131" s="19"/>
       <c r="C131" s="19"/>
-      <c r="D131" s="19"/>
-      <c r="E131" s="19"/>
-      <c r="F131" s="19"/>
-      <c r="G131" s="19"/>
-      <c r="H131" s="22"/>
-    </row>
-    <row r="132" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D131" s="19" t="s">
+        <v>370</v>
+      </c>
+      <c r="E131" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F131" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="G131" s="31" t="s">
+        <v>373</v>
+      </c>
+      <c r="H131" s="22" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" s="21" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="7">
         <v>131</v>
       </c>
       <c r="B132" s="19"/>
-      <c r="C132" s="19"/>
+      <c r="C132" s="19" t="s">
+        <v>375</v>
+      </c>
       <c r="D132" s="19"/>
       <c r="E132" s="19"/>
-      <c r="F132" s="19"/>
+      <c r="F132" s="19" t="s">
+        <v>376</v>
+      </c>
       <c r="G132" s="19"/>
-      <c r="H132" s="22"/>
+      <c r="H132" s="22" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="133" spans="1:8" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="7">
@@ -5160,9 +5269,15 @@
       </c>
       <c r="B133" s="19"/>
       <c r="C133" s="19"/>
-      <c r="D133" s="19"/>
-      <c r="E133" s="19"/>
-      <c r="F133" s="19"/>
+      <c r="D133" s="19" t="s">
+        <v>377</v>
+      </c>
+      <c r="E133" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F133" s="19" t="s">
+        <v>378</v>
+      </c>
       <c r="G133" s="19"/>
       <c r="H133" s="22"/>
     </row>

</xml_diff>